<commit_message>
rename superimposition to superposition; edit manuscript to nearly complete intro and methods
</commit_message>
<xml_diff>
--- a/QTY Design/Protein info.xlsx
+++ b/QTY Design/Protein info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\Rhodopsins_QTY\QTY Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D37F46D-89D1-4089-86CA-922D56A96093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5884F050-3EEC-477F-BD8F-D938AA85417A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="6765" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>

</xml_diff>